<commit_message>
Added Hashmat the brave
</commit_message>
<xml_diff>
--- a/Project100_complete-syllabus.xlsx
+++ b/Project100_complete-syllabus.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -536,8 +536,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -631,8 +631,16 @@
       <name val="Georgia"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -657,8 +665,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -729,11 +742,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -840,8 +869,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -900,7 +939,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -932,9 +971,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -966,6 +1006,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1141,944 +1182,944 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B155"/>
   <sheetViews>
     <sheetView topLeftCell="A88" workbookViewId="0">
       <selection activeCell="B126" sqref="B126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="60.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" customWidth="1"/>
+    <col min="2" max="2" width="60.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1">
+    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1">
+    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1">
+    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1">
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1">
+    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1">
+    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1">
+    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1">
+    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1">
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" thickBot="1">
+    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1">
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1">
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1">
+    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1">
+    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" thickBot="1">
+    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1">
+    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1">
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" thickBot="1">
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" thickBot="1">
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" thickBot="1">
+    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" thickBot="1">
+    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" thickBot="1">
+    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" thickBot="1">
+    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1">
+    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" thickBot="1">
+    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" thickBot="1">
+    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" thickBot="1">
+    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" thickBot="1">
+    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="B29" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" thickBot="1">
+    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="B30" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="27" thickBot="1">
+    <row r="31" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" thickBot="1">
+    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75" thickBot="1">
+    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
       <c r="B33" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.75" thickBot="1">
+    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
       <c r="B34" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.75" thickBot="1">
+    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="B35" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.75" thickBot="1">
+    <row r="36" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="1:2" ht="15.75" thickBot="1">
+    <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
       <c r="B37" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15.75" thickBot="1">
+    <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
       <c r="B38" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15.75" thickBot="1">
+    <row r="39" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="B39" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15.75" thickBot="1">
+    <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
       <c r="B40" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15.75" thickBot="1">
+    <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
       <c r="B41" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15.75" thickBot="1">
+    <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2"/>
       <c r="B42" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15.75" thickBot="1">
+    <row r="43" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
       <c r="B43" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15.75" thickBot="1">
+    <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2"/>
       <c r="B44" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15.75" thickBot="1">
+    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2"/>
       <c r="B45" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15.75" thickBot="1">
+    <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
       <c r="B46" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15.75" thickBot="1">
+    <row r="47" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
       <c r="B47" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15.75" thickBot="1">
+    <row r="48" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2"/>
       <c r="B48" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.75" thickBot="1">
+    <row r="49" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="2"/>
       <c r="B49" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.75" thickBot="1">
+    <row r="50" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2"/>
       <c r="B50" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15.75" thickBot="1">
+    <row r="51" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="2"/>
       <c r="B51" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15.75" thickBot="1">
+    <row r="52" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2"/>
       <c r="B52" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15.75" thickBot="1">
+    <row r="53" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="2"/>
       <c r="B53" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15.75" thickBot="1">
+    <row r="54" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
       <c r="B54" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15.75" thickBot="1">
+    <row r="55" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="2"/>
       <c r="B55" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15.75" thickBot="1">
+    <row r="56" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="2"/>
       <c r="B56" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15.75" thickBot="1">
+    <row r="57" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="2"/>
       <c r="B57" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15.75" thickBot="1">
+    <row r="58" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="2"/>
       <c r="B58" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15.75" thickBot="1">
+    <row r="59" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="2"/>
       <c r="B59" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15.75" thickBot="1">
+    <row r="60" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="2"/>
       <c r="B60" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15.75" thickBot="1">
+    <row r="61" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="2"/>
       <c r="B61" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="15.75" thickBot="1">
+    <row r="62" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="2"/>
       <c r="B62" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15.75" thickBot="1">
+    <row r="63" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="2"/>
       <c r="B63" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15.75" thickBot="1">
+    <row r="64" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="2"/>
       <c r="B64" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="15.75" thickBot="1">
+    <row r="65" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="2"/>
       <c r="B65" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15.75" thickBot="1">
+    <row r="66" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="2"/>
       <c r="B66" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15.75" thickBot="1">
+    <row r="67" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="2"/>
       <c r="B67" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="15.75" thickBot="1">
+    <row r="68" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="2"/>
       <c r="B68" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15.75" thickBot="1">
+    <row r="69" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="2"/>
       <c r="B69" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="15.75" thickBot="1">
+    <row r="70" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="2"/>
       <c r="B70" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="15.75" thickBot="1">
+    <row r="71" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="2"/>
       <c r="B71" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15.75" thickBot="1">
+    <row r="72" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="2"/>
       <c r="B72" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="27" thickBot="1">
+    <row r="73" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="2"/>
       <c r="B73" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15.75" thickBot="1">
+    <row r="74" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="2"/>
       <c r="B74" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="15.75" thickBot="1">
+    <row r="75" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="2"/>
       <c r="B75" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15.75" thickBot="1">
+    <row r="76" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="2"/>
       <c r="B76" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15.75" thickBot="1">
+    <row r="77" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B77" s="2"/>
     </row>
-    <row r="78" spans="1:2" ht="15.75" thickBot="1">
+    <row r="78" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="2"/>
       <c r="B78" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15.75" thickBot="1">
+    <row r="79" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="2"/>
       <c r="B79" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="15.75" thickBot="1">
+    <row r="80" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="2"/>
       <c r="B80" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="15.75" thickBot="1">
+    <row r="81" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="2"/>
       <c r="B81" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="15.75" thickBot="1">
+    <row r="82" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B82" s="2"/>
     </row>
-    <row r="83" spans="1:2" ht="15.75" thickBot="1">
+    <row r="83" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="2"/>
       <c r="B83" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="15.75" thickBot="1">
+    <row r="84" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
       <c r="B84" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="15.75" thickBot="1">
+    <row r="85" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="2"/>
       <c r="B85" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="15.75" thickBot="1">
+    <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="2"/>
       <c r="B86" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="15.75" thickBot="1">
+    <row r="87" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="2"/>
       <c r="B87" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="15.75" thickBot="1">
+    <row r="88" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="2"/>
       <c r="B88" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="15.75" thickBot="1">
+    <row r="89" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="2"/>
       <c r="B89" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="15.75" thickBot="1">
+    <row r="90" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="2"/>
       <c r="B90" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="15.75" thickBot="1">
+    <row r="91" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B91" s="2"/>
     </row>
-    <row r="92" spans="1:2" ht="15.75" thickBot="1">
+    <row r="92" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="2"/>
       <c r="B92" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="15.75" thickBot="1">
+    <row r="93" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="2"/>
       <c r="B93" s="6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="15.75" thickBot="1">
+    <row r="94" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="2"/>
       <c r="B94" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="15.75" thickBot="1">
+    <row r="95" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
       <c r="B95" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="15.75" thickBot="1">
+    <row r="96" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="2"/>
       <c r="B96" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="15.75" thickBot="1">
+    <row r="97" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="2"/>
       <c r="B97" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="15.75" thickBot="1">
+    <row r="98" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="2"/>
       <c r="B98" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="15.75" thickBot="1">
+    <row r="99" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="2"/>
       <c r="B99" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="15.75" thickBot="1">
+    <row r="100" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="2"/>
       <c r="B100" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="15.75" thickBot="1">
+    <row r="101" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="2"/>
       <c r="B101" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="15.75" thickBot="1">
+    <row r="102" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="2"/>
       <c r="B102" s="6" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="15.75" thickBot="1">
+    <row r="103" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="2"/>
       <c r="B103" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="15.75" thickBot="1">
+    <row r="104" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="2"/>
       <c r="B104" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="15.75" thickBot="1">
+    <row r="105" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="2"/>
       <c r="B105" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="15.75" thickBot="1">
+    <row r="106" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="2"/>
       <c r="B106" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="15.75" thickBot="1">
+    <row r="107" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="2"/>
       <c r="B107" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="15.75" thickBot="1">
+    <row r="108" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="2"/>
       <c r="B108" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="15.75" thickBot="1">
+    <row r="109" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="2"/>
       <c r="B109" s="6" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="15.75" thickBot="1">
+    <row r="110" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="2"/>
       <c r="B110" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="15.75" thickBot="1">
+    <row r="111" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B111" s="2"/>
     </row>
-    <row r="112" spans="1:2" ht="15.75" thickBot="1">
+    <row r="112" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="2"/>
       <c r="B112" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="15.75" thickBot="1">
+    <row r="113" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="2"/>
       <c r="B113" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="15.75" thickBot="1">
+    <row r="114" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="2"/>
       <c r="B114" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="15.75" thickBot="1">
+    <row r="115" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="2"/>
       <c r="B115" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="15.75" thickBot="1">
+    <row r="116" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="2"/>
       <c r="B116" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="15.75" thickBot="1">
+    <row r="117" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="2"/>
       <c r="B117" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="15.75" thickBot="1">
+    <row r="118" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="2"/>
       <c r="B118" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="15.75" thickBot="1">
+    <row r="119" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="2"/>
       <c r="B119" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="15.75" thickBot="1">
+    <row r="120" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="2"/>
       <c r="B120" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="15.75" thickBot="1">
+    <row r="121" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="2"/>
       <c r="B121" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="15.75" thickBot="1">
+    <row r="122" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="2"/>
       <c r="B122" s="6" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="15.75" thickBot="1">
+    <row r="123" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="2"/>
       <c r="B123" s="6" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="15.75" thickBot="1">
+    <row r="124" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="2"/>
       <c r="B124" s="6" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="15.75" thickBot="1">
+    <row r="125" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B125" s="2"/>
     </row>
-    <row r="126" spans="1:2" ht="15.75" thickBot="1">
+    <row r="126" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="2"/>
       <c r="B126" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="15.75" thickBot="1">
+    <row r="127" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="2"/>
       <c r="B127" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="15.75" thickBot="1">
+    <row r="128" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="2"/>
       <c r="B128" s="6" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="15.75" thickBot="1">
+    <row r="129" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="2"/>
       <c r="B129" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="15.75" thickBot="1">
+    <row r="130" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B130" s="2"/>
     </row>
-    <row r="131" spans="1:2" ht="15.75" thickBot="1">
+    <row r="131" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="2"/>
       <c r="B131" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="15.75" thickBot="1">
+    <row r="132" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A132" s="2"/>
       <c r="B132" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="15.75" thickBot="1">
+    <row r="133" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A133" s="2"/>
       <c r="B133" s="6" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="15.75" thickBot="1">
+    <row r="134" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A134" s="2"/>
       <c r="B134" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="15.75" thickBot="1">
+    <row r="135" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A135" s="2"/>
       <c r="B135" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="15.75" thickBot="1">
+    <row r="136" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B136" s="2"/>
     </row>
-    <row r="137" spans="1:2" ht="15.75" thickBot="1">
+    <row r="137" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A137" s="2"/>
       <c r="B137" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="15.75" thickBot="1">
+    <row r="138" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A138" s="2"/>
       <c r="B138" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="15.75" thickBot="1">
+    <row r="139" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A139" s="2"/>
       <c r="B139" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="15.75" thickBot="1">
+    <row r="140" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="2"/>
       <c r="B140" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="15.75" thickBot="1">
+    <row r="141" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="2"/>
       <c r="B141" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="15.75" thickBot="1">
+    <row r="142" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A142" s="2"/>
       <c r="B142" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="15.75" thickBot="1">
+    <row r="143" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="2"/>
       <c r="B143" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="15.75" thickBot="1">
+    <row r="144" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A144" s="2"/>
       <c r="B144" s="6" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="15.75" thickBot="1">
+    <row r="145" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="2"/>
       <c r="B145" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="15.75" thickBot="1">
+    <row r="146" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="2"/>
       <c r="B146" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="15.75" thickBot="1">
+    <row r="147" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A147" s="2"/>
       <c r="B147" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="15.75" thickBot="1">
+    <row r="148" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A148" s="2"/>
       <c r="B148" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="15.75" thickBot="1">
+    <row r="149" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A149" s="2"/>
       <c r="B149" s="8" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="15.75" thickBot="1">
+    <row r="150" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A150" s="2"/>
       <c r="B150" s="6" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="15.75" thickBot="1">
+    <row r="151" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A151" s="2"/>
       <c r="B151" s="6" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="15.75" thickBot="1">
+    <row r="152" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A152" s="2"/>
       <c r="B152" s="6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="15.75" thickBot="1">
+    <row r="153" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A153" s="2"/>
       <c r="B153" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="15.75" thickBot="1">
+    <row r="154" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A154" s="2"/>
       <c r="B154" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="15.75" thickBot="1">
+    <row r="155" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A155" s="2"/>
       <c r="B155" s="3" t="s">
         <v>154</v>
@@ -2091,23 +2132,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C34" activeCellId="2" sqref="C30:C32 C33 C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="61.5703125" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
-    <col min="6" max="6" width="67.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="3" max="3" width="61.5546875" customWidth="1"/>
+    <col min="5" max="5" width="26.109375" customWidth="1"/>
+    <col min="6" max="6" width="67.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="23.25">
+    <row r="1" spans="2:7" ht="23.4" x14ac:dyDescent="0.3">
       <c r="C1" s="41" t="s">
         <v>159</v>
       </c>
@@ -2115,7 +2156,7 @@
       <c r="E1" s="41"/>
       <c r="F1" s="41"/>
     </row>
-    <row r="3" spans="2:7" ht="18.75">
+    <row r="3" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B3" s="39" t="s">
         <v>155</v>
       </c>
@@ -2127,19 +2168,20 @@
       <c r="F3" s="39"/>
       <c r="G3" s="39"/>
     </row>
-    <row r="5" spans="2:7" ht="16.5" customHeight="1">
-      <c r="B5" s="12" t="s">
+    <row r="4" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="2:7" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="13"/>
+      <c r="C5" s="43"/>
       <c r="E5" s="12" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="2:7">
-      <c r="B6" s="13"/>
-      <c r="C6" s="15" t="s">
+    <row r="6" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="43"/>
+      <c r="C6" s="44" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="16"/>
@@ -2147,9 +2189,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:7">
-      <c r="B7" s="13"/>
-      <c r="C7" s="14" t="s">
+    <row r="7" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="43"/>
+      <c r="C7" s="44" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="16"/>
@@ -2157,9 +2199,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="2:7">
-      <c r="B8" s="13"/>
-      <c r="C8" s="14" t="s">
+    <row r="8" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="43"/>
+      <c r="C8" s="44" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="16"/>
@@ -2167,9 +2209,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="13"/>
-      <c r="C9" s="14" t="s">
+    <row r="9" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="43"/>
+      <c r="C9" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="16"/>
@@ -2177,21 +2219,21 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="2:7">
-      <c r="B10" s="13"/>
-      <c r="C10" s="14" t="s">
+    <row r="10" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="43"/>
+      <c r="C10" s="44" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:7">
-      <c r="B11" s="13"/>
-      <c r="C11" s="14" t="s">
+    <row r="11" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="43"/>
+      <c r="C11" s="44" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:7">
-      <c r="B12" s="13"/>
-      <c r="C12" s="14" t="s">
+    <row r="12" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="43"/>
+      <c r="C12" s="44" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="12" t="s">
@@ -2199,9 +2241,9 @@
       </c>
       <c r="F12" s="13"/>
     </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="13"/>
-      <c r="C13" s="14" t="s">
+    <row r="13" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="43"/>
+      <c r="C13" s="44" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="13"/>
@@ -2209,9 +2251,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="2:7">
-      <c r="B14" s="13"/>
-      <c r="C14" s="14" t="s">
+    <row r="14" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="43"/>
+      <c r="C14" s="44" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="13"/>
@@ -2219,9 +2261,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="2:7">
-      <c r="B15" s="13"/>
-      <c r="C15" s="14" t="s">
+    <row r="15" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="43"/>
+      <c r="C15" s="44" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="13"/>
@@ -2229,9 +2271,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="2:7">
-      <c r="B16" s="13"/>
-      <c r="C16" s="14" t="s">
+    <row r="16" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="43"/>
+      <c r="C16" s="44" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="13"/>
@@ -2239,9 +2281,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="13"/>
-      <c r="C17" s="14" t="s">
+    <row r="17" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="43"/>
+      <c r="C17" s="44" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="13"/>
@@ -2249,25 +2291,25 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E18" s="13"/>
       <c r="F18" s="15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="26.25">
-      <c r="B19" s="12" t="s">
+    <row r="19" spans="2:6" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="13"/>
+      <c r="C19" s="43"/>
       <c r="E19" s="16"/>
       <c r="F19" s="15" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
-      <c r="B20" s="13"/>
-      <c r="C20" s="14" t="s">
+    <row r="20" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="43"/>
+      <c r="C20" s="44" t="s">
         <v>14</v>
       </c>
       <c r="E20" s="16"/>
@@ -2275,9 +2317,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
-      <c r="B21" s="13"/>
-      <c r="C21" s="14" t="s">
+    <row r="21" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="43"/>
+      <c r="C21" s="44" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="16"/>
@@ -2285,15 +2327,15 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B22" s="13"/>
-      <c r="C22" s="14" t="s">
+    <row r="22" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="43"/>
+      <c r="C22" s="44" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B23" s="13"/>
-      <c r="C23" s="14" t="s">
+    <row r="23" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="43"/>
+      <c r="C23" s="44" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="1" t="s">
@@ -2301,9 +2343,9 @@
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B24" s="13"/>
-      <c r="C24" s="14" t="s">
+    <row r="24" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="43"/>
+      <c r="C24" s="44" t="s">
         <v>18</v>
       </c>
       <c r="E24" s="2"/>
@@ -2311,9 +2353,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B25" s="13"/>
-      <c r="C25" s="14" t="s">
+    <row r="25" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="43"/>
+      <c r="C25" s="44" t="s">
         <v>21</v>
       </c>
       <c r="E25" s="2"/>
@@ -2321,9 +2363,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B26" s="13"/>
-      <c r="C26" s="14" t="s">
+    <row r="26" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="43"/>
+      <c r="C26" s="44" t="s">
         <v>22</v>
       </c>
       <c r="E26" s="2"/>
@@ -2331,9 +2373,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B27" s="13"/>
-      <c r="C27" s="14" t="s">
+    <row r="27" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="43"/>
+      <c r="C27" s="44" t="s">
         <v>23</v>
       </c>
       <c r="E27" s="2"/>
@@ -2341,10 +2383,10 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="15.75" thickBot="1">
+    <row r="28" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="17"/>
     </row>
-    <row r="29" spans="2:6" ht="15.75" thickBot="1">
+    <row r="29" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="12" t="s">
         <v>35</v>
       </c>
@@ -2354,9 +2396,9 @@
       </c>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" ht="15.75" thickBot="1">
+    <row r="30" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="13"/>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="44" t="s">
         <v>36</v>
       </c>
       <c r="E30" s="2"/>
@@ -2364,9 +2406,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="15.75" thickBot="1">
+    <row r="31" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="13"/>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="44" t="s">
         <v>37</v>
       </c>
       <c r="E31" s="2"/>
@@ -2374,9 +2416,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="19.5" thickBot="1">
+    <row r="32" spans="2:6" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="13"/>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="44" t="s">
         <v>38</v>
       </c>
       <c r="D32" s="9"/>
@@ -2385,9 +2427,9 @@
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="15.75" customHeight="1" thickBot="1">
+    <row r="33" spans="2:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="13"/>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="44" t="s">
         <v>39</v>
       </c>
       <c r="E33" s="2"/>
@@ -2395,14 +2437,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="15.75" thickBot="1">
+    <row r="34" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="13"/>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="44" t="s">
         <v>40</v>
       </c>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="2:6">
+    <row r="35" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B35" s="13"/>
       <c r="C35" s="14" t="s">
         <v>41</v>
@@ -2412,7 +2454,7 @@
       </c>
       <c r="F35" s="13"/>
     </row>
-    <row r="36" spans="2:6">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="13"/>
       <c r="C36" s="14" t="s">
         <v>42</v>
@@ -2422,7 +2464,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="2:6">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="13"/>
       <c r="C37" s="14" t="s">
         <v>43</v>
@@ -2432,7 +2474,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="2:6">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" s="13"/>
       <c r="C38" s="14" t="s">
         <v>44</v>
@@ -2442,7 +2484,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="2:6">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="13"/>
       <c r="C39" s="14" t="s">
         <v>45</v>
@@ -2452,7 +2494,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="2:6">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="13"/>
       <c r="C40" s="14" t="s">
         <v>46</v>
@@ -2462,7 +2504,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="2:6">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="13"/>
       <c r="C41" s="14" t="s">
         <v>47</v>
@@ -2472,7 +2514,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="2:6">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="13"/>
       <c r="C42" s="14" t="s">
         <v>48</v>
@@ -2482,7 +2524,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="2:6">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="13"/>
       <c r="C43" s="14" t="s">
         <v>49</v>
@@ -2492,19 +2534,19 @@
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="2:6" ht="15.75" thickBot="1">
+    <row r="44" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B44" s="13"/>
       <c r="C44" s="14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="2:6" ht="27" thickBot="1">
+    <row r="45" spans="2:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B45" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="2:6" ht="15.75" thickBot="1">
+    <row r="46" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="2"/>
       <c r="C46" s="4" t="s">
         <v>82</v>
@@ -2516,7 +2558,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="47" spans="2:6" ht="19.5" customHeight="1" thickBot="1">
+    <row r="47" spans="2:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B47" s="2"/>
       <c r="C47" s="4" t="s">
         <v>83</v>
@@ -2528,7 +2570,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="48" spans="2:6" ht="15.75" thickBot="1">
+    <row r="48" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B48" s="2"/>
       <c r="C48" s="4" t="s">
         <v>84</v>
@@ -2536,13 +2578,13 @@
       <c r="E48" s="10"/>
       <c r="F48" s="11"/>
     </row>
-    <row r="49" spans="2:7" ht="15.75" thickBot="1">
+    <row r="49" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B49" s="2"/>
       <c r="C49" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="2:7">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B51" s="33" t="s">
         <v>164</v>
       </c>
@@ -2550,7 +2592,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="52" spans="2:7">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B52" s="35" t="s">
         <v>165</v>
       </c>
@@ -2558,7 +2600,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="2:7" ht="18.75">
+    <row r="55" spans="2:7" ht="18" x14ac:dyDescent="0.35">
       <c r="B55" s="39" t="s">
         <v>157</v>
       </c>
@@ -2569,7 +2611,7 @@
       <c r="F55" s="40"/>
       <c r="G55" s="40"/>
     </row>
-    <row r="56" spans="2:7">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B56" s="12" t="s">
         <v>124</v>
       </c>
@@ -2579,7 +2621,7 @@
       </c>
       <c r="F56" s="16"/>
     </row>
-    <row r="57" spans="2:7">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B57" s="13"/>
       <c r="C57" s="15" t="s">
         <v>125</v>
@@ -2589,7 +2631,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="2:7">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B58" s="13"/>
       <c r="C58" s="14" t="s">
         <v>126</v>
@@ -2599,7 +2641,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="2:7" ht="26.25">
+    <row r="59" spans="2:7" ht="27" x14ac:dyDescent="0.3">
       <c r="B59" s="13"/>
       <c r="C59" s="19" t="s">
         <v>127</v>
@@ -2609,7 +2651,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="2:7">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B60" s="13"/>
       <c r="C60" s="14" t="s">
         <v>128</v>
@@ -2619,7 +2661,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="2:7" ht="26.25">
+    <row r="61" spans="2:7" ht="27" x14ac:dyDescent="0.3">
       <c r="B61" s="16"/>
       <c r="C61" s="15" t="s">
         <v>72</v>
@@ -2629,25 +2671,25 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="2:7" ht="15.75" thickBot="1">
+    <row r="62" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E62" s="16"/>
       <c r="F62" s="18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="63" spans="2:7" ht="15.75" thickBot="1">
+    <row r="63" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B63" s="1" t="s">
         <v>129</v>
       </c>
       <c r="C63" s="2"/>
     </row>
-    <row r="64" spans="2:7" ht="15.75" thickBot="1">
+    <row r="64" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B64" s="2"/>
       <c r="C64" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="65" spans="2:6" ht="15.75" thickBot="1">
+    <row r="65" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B65" s="2"/>
       <c r="C65" s="20" t="s">
         <v>131</v>
@@ -2657,7 +2699,7 @@
       </c>
       <c r="F65" s="16"/>
     </row>
-    <row r="66" spans="2:6" ht="15.75" thickBot="1">
+    <row r="66" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B66" s="2"/>
       <c r="C66" s="20" t="s">
         <v>132</v>
@@ -2667,7 +2709,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="2:6" ht="15.75" thickBot="1">
+    <row r="67" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B67" s="2"/>
       <c r="C67" s="4" t="s">
         <v>133</v>
@@ -2677,7 +2719,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="2:6" ht="15.75" thickBot="1">
+    <row r="68" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B68" s="2"/>
       <c r="C68" s="4" t="s">
         <v>134</v>
@@ -2687,13 +2729,13 @@
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="2:6" ht="15.75" thickBot="1">
+    <row r="69" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E69" s="16"/>
       <c r="F69" s="25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="2:6" ht="15.75" thickBot="1">
+    <row r="70" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B70" s="1" t="s">
         <v>135</v>
       </c>
@@ -2703,7 +2745,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="71" spans="2:6" ht="15.75" thickBot="1">
+    <row r="71" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B71" s="2"/>
       <c r="C71" s="4" t="s">
         <v>136</v>
@@ -2713,7 +2755,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="72" spans="2:6" ht="15.75" thickBot="1">
+    <row r="72" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B72" s="2"/>
       <c r="C72" s="4" t="s">
         <v>137</v>
@@ -2723,7 +2765,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="73" spans="2:6" ht="15.75" thickBot="1">
+    <row r="73" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B73" s="2"/>
       <c r="C73" s="20" t="s">
         <v>138</v>
@@ -2733,7 +2775,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="2:6" ht="15.75" thickBot="1">
+    <row r="74" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B74" s="2"/>
       <c r="C74" s="20" t="s">
         <v>139</v>
@@ -2743,7 +2785,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="75" spans="2:6" ht="15.75" thickBot="1">
+    <row r="75" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B75" s="2"/>
       <c r="C75" s="20" t="s">
         <v>140</v>
@@ -2753,7 +2795,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="76" spans="2:6" ht="15.75" thickBot="1">
+    <row r="76" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B76" s="2"/>
       <c r="C76" s="20" t="s">
         <v>141</v>
@@ -2763,7 +2805,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="77" spans="2:6" ht="15.75" thickBot="1">
+    <row r="77" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B77" s="2"/>
       <c r="C77" s="20" t="s">
         <v>142</v>
@@ -2773,7 +2815,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="78" spans="2:6" ht="15.75" thickBot="1">
+    <row r="78" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B78" s="2"/>
       <c r="C78" s="20" t="s">
         <v>143</v>
@@ -2783,7 +2825,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="2:6" ht="15.75" thickBot="1">
+    <row r="79" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B79" s="2"/>
       <c r="C79" s="20" t="s">
         <v>144</v>
@@ -2793,13 +2835,13 @@
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="2:6" ht="15.75" thickBot="1">
+    <row r="80" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B80" s="2"/>
       <c r="C80" s="20" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="81" spans="2:6" ht="15.75" thickBot="1">
+    <row r="81" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B81" s="2"/>
       <c r="C81" s="20" t="s">
         <v>146</v>
@@ -2809,7 +2851,7 @@
       </c>
       <c r="F81" s="16"/>
     </row>
-    <row r="82" spans="2:6" ht="15.75" thickBot="1">
+    <row r="82" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B82" s="2"/>
       <c r="C82" s="20" t="s">
         <v>147</v>
@@ -2819,7 +2861,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="83" spans="2:6" ht="15.75" thickBot="1">
+    <row r="83" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B83" s="2"/>
       <c r="C83" s="20" t="s">
         <v>148</v>
@@ -2829,7 +2871,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="2:6" ht="15.75" thickBot="1">
+    <row r="84" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B84" s="2"/>
       <c r="C84" s="20" t="s">
         <v>149</v>
@@ -2839,7 +2881,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="85" spans="2:6" ht="15.75" thickBot="1">
+    <row r="85" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B85" s="2"/>
       <c r="C85" s="20" t="s">
         <v>150</v>
@@ -2849,7 +2891,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="86" spans="2:6" ht="15.75" thickBot="1">
+    <row r="86" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B86" s="2"/>
       <c r="C86" s="20" t="s">
         <v>151</v>
@@ -2859,7 +2901,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="87" spans="2:6" ht="15.75" thickBot="1">
+    <row r="87" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B87" s="2"/>
       <c r="C87" s="4" t="s">
         <v>152</v>
@@ -2869,7 +2911,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="88" spans="2:6" ht="15.75" thickBot="1">
+    <row r="88" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B88" s="2"/>
       <c r="C88" s="4" t="s">
         <v>153</v>
@@ -2879,7 +2921,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="89" spans="2:6" ht="15.75" thickBot="1">
+    <row r="89" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B89" s="2"/>
       <c r="C89" s="3" t="s">
         <v>154</v>
@@ -2889,7 +2931,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="90" spans="2:6" ht="15.75">
+    <row r="90" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B90" s="36" t="s">
         <v>168</v>
       </c>
@@ -2901,13 +2943,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="91" spans="2:6">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E91" s="16"/>
       <c r="F91" s="25" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="92" spans="2:6">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B92" s="21" t="s">
         <v>90</v>
       </c>
@@ -2917,7 +2959,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="93" spans="2:6">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B93" s="22"/>
       <c r="C93" s="23" t="s">
         <v>91</v>
@@ -2927,7 +2969,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="94" spans="2:6">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B94" s="22"/>
       <c r="C94" s="23"/>
       <c r="E94" s="16"/>
@@ -2935,7 +2977,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="95" spans="2:6">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B95" s="22"/>
       <c r="C95" s="23" t="s">
         <v>93</v>
@@ -2944,7 +2986,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="96" spans="2:6">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B96" s="22"/>
       <c r="C96" s="23" t="s">
         <v>94</v>
@@ -2956,59 +2998,59 @@
         <v>163</v>
       </c>
     </row>
-    <row r="97" spans="2:3">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B97" s="22"/>
       <c r="C97" s="23" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="2:3">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B98" s="22"/>
       <c r="C98" s="23" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="2:3">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B99" s="22"/>
       <c r="C99" s="23" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="2:3">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B100" s="22"/>
       <c r="C100" s="23" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="2:3">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B101" s="22"/>
       <c r="C101" s="23" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="2:3">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B102" s="22"/>
       <c r="C102" s="23" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="103" spans="2:3">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B103" s="22"/>
       <c r="C103" s="23" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="104" spans="2:3">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B104" s="27"/>
       <c r="C104" s="28" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="105" spans="2:3">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B105" s="32"/>
       <c r="C105" s="26"/>
     </row>
-    <row r="106" spans="2:3">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B106" s="33" t="s">
         <v>164</v>
       </c>
@@ -3016,19 +3058,19 @@
         <v>162</v>
       </c>
     </row>
-    <row r="107" spans="2:3">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B107" s="29"/>
       <c r="C107" s="11"/>
     </row>
-    <row r="108" spans="2:3">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B108" s="29"/>
       <c r="C108" s="11"/>
     </row>
-    <row r="109" spans="2:3">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B109" s="29"/>
       <c r="C109" s="30"/>
     </row>
-    <row r="110" spans="2:3">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B110" s="31"/>
       <c r="C110" s="31"/>
     </row>

</xml_diff>

<commit_message>
Added some problems and solved Hashmat The Brave Warrior in 0.000 seconds
</commit_message>
<xml_diff>
--- a/Project100_complete-syllabus.xlsx
+++ b/Project100_complete-syllabus.xlsx
@@ -860,6 +860,15 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -868,15 +877,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2136,7 +2136,7 @@
   <dimension ref="B1:G110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C34" activeCellId="2" sqref="C30:C32 C33 C34"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2149,39 +2149,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="44" t="s">
         <v>159</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
     </row>
     <row r="3" spans="2:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="C3" s="39"/>
+      <c r="C3" s="42"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
     </row>
     <row r="4" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:7" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="43"/>
+      <c r="C5" s="40"/>
       <c r="E5" s="12" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="13"/>
     </row>
     <row r="6" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="43"/>
-      <c r="C6" s="44" t="s">
+      <c r="B6" s="40"/>
+      <c r="C6" s="41" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="16"/>
@@ -2190,8 +2190,8 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="43"/>
-      <c r="C7" s="44" t="s">
+      <c r="B7" s="40"/>
+      <c r="C7" s="41" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="16"/>
@@ -2200,8 +2200,8 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="43"/>
-      <c r="C8" s="44" t="s">
+      <c r="B8" s="40"/>
+      <c r="C8" s="41" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="16"/>
@@ -2210,8 +2210,8 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="43"/>
-      <c r="C9" s="44" t="s">
+      <c r="B9" s="40"/>
+      <c r="C9" s="41" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="16"/>
@@ -2220,20 +2220,20 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="43"/>
-      <c r="C10" s="44" t="s">
+      <c r="B10" s="40"/>
+      <c r="C10" s="41" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="43"/>
-      <c r="C11" s="44" t="s">
+      <c r="B11" s="40"/>
+      <c r="C11" s="41" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="43"/>
-      <c r="C12" s="44" t="s">
+      <c r="B12" s="40"/>
+      <c r="C12" s="41" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="12" t="s">
@@ -2242,8 +2242,8 @@
       <c r="F12" s="13"/>
     </row>
     <row r="13" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="43"/>
-      <c r="C13" s="44" t="s">
+      <c r="B13" s="40"/>
+      <c r="C13" s="41" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="13"/>
@@ -2252,8 +2252,8 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="43"/>
-      <c r="C14" s="44" t="s">
+      <c r="B14" s="40"/>
+      <c r="C14" s="41" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="13"/>
@@ -2262,8 +2262,8 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="43"/>
-      <c r="C15" s="44" t="s">
+      <c r="B15" s="40"/>
+      <c r="C15" s="41" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="13"/>
@@ -2272,8 +2272,8 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="43"/>
-      <c r="C16" s="44" t="s">
+      <c r="B16" s="40"/>
+      <c r="C16" s="41" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="13"/>
@@ -2282,8 +2282,8 @@
       </c>
     </row>
     <row r="17" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="43"/>
-      <c r="C17" s="44" t="s">
+      <c r="B17" s="40"/>
+      <c r="C17" s="41" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="13"/>
@@ -2298,18 +2298,18 @@
       </c>
     </row>
     <row r="19" spans="2:6" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="43"/>
+      <c r="C19" s="40"/>
       <c r="E19" s="16"/>
       <c r="F19" s="15" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="43"/>
-      <c r="C20" s="44" t="s">
+      <c r="B20" s="40"/>
+      <c r="C20" s="41" t="s">
         <v>14</v>
       </c>
       <c r="E20" s="16"/>
@@ -2318,8 +2318,8 @@
       </c>
     </row>
     <row r="21" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="43"/>
-      <c r="C21" s="44" t="s">
+      <c r="B21" s="40"/>
+      <c r="C21" s="41" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="16"/>
@@ -2328,14 +2328,14 @@
       </c>
     </row>
     <row r="22" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="43"/>
-      <c r="C22" s="44" t="s">
+      <c r="B22" s="40"/>
+      <c r="C22" s="41" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="43"/>
-      <c r="C23" s="44" t="s">
+      <c r="B23" s="40"/>
+      <c r="C23" s="41" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="1" t="s">
@@ -2344,8 +2344,8 @@
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="43"/>
-      <c r="C24" s="44" t="s">
+      <c r="B24" s="40"/>
+      <c r="C24" s="41" t="s">
         <v>18</v>
       </c>
       <c r="E24" s="2"/>
@@ -2354,8 +2354,8 @@
       </c>
     </row>
     <row r="25" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="43"/>
-      <c r="C25" s="44" t="s">
+      <c r="B25" s="40"/>
+      <c r="C25" s="41" t="s">
         <v>21</v>
       </c>
       <c r="E25" s="2"/>
@@ -2364,8 +2364,8 @@
       </c>
     </row>
     <row r="26" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="43"/>
-      <c r="C26" s="44" t="s">
+      <c r="B26" s="40"/>
+      <c r="C26" s="41" t="s">
         <v>22</v>
       </c>
       <c r="E26" s="2"/>
@@ -2374,8 +2374,8 @@
       </c>
     </row>
     <row r="27" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="43"/>
-      <c r="C27" s="44" t="s">
+      <c r="B27" s="40"/>
+      <c r="C27" s="41" t="s">
         <v>23</v>
       </c>
       <c r="E27" s="2"/>
@@ -2398,7 +2398,7 @@
     </row>
     <row r="30" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="13"/>
-      <c r="C30" s="44" t="s">
+      <c r="C30" s="41" t="s">
         <v>36</v>
       </c>
       <c r="E30" s="2"/>
@@ -2408,7 +2408,7 @@
     </row>
     <row r="31" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="13"/>
-      <c r="C31" s="44" t="s">
+      <c r="C31" s="41" t="s">
         <v>37</v>
       </c>
       <c r="E31" s="2"/>
@@ -2418,7 +2418,7 @@
     </row>
     <row r="32" spans="2:6" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="13"/>
-      <c r="C32" s="44" t="s">
+      <c r="C32" s="41" t="s">
         <v>38</v>
       </c>
       <c r="D32" s="9"/>
@@ -2429,7 +2429,7 @@
     </row>
     <row r="33" spans="2:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="13"/>
-      <c r="C33" s="44" t="s">
+      <c r="C33" s="41" t="s">
         <v>39</v>
       </c>
       <c r="E33" s="2"/>
@@ -2439,14 +2439,14 @@
     </row>
     <row r="34" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="13"/>
-      <c r="C34" s="44" t="s">
+      <c r="C34" s="41" t="s">
         <v>40</v>
       </c>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="13"/>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="41" t="s">
         <v>41</v>
       </c>
       <c r="E35" s="12" t="s">
@@ -2454,7 +2454,7 @@
       </c>
       <c r="F35" s="13"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B36" s="13"/>
       <c r="C36" s="14" t="s">
         <v>42</v>
@@ -2601,15 +2601,15 @@
       </c>
     </row>
     <row r="55" spans="2:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="B55" s="39" t="s">
+      <c r="B55" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="C55" s="39"/>
-      <c r="E55" s="39" t="s">
+      <c r="C55" s="42"/>
+      <c r="E55" s="42" t="s">
         <v>158</v>
       </c>
-      <c r="F55" s="40"/>
-      <c r="G55" s="40"/>
+      <c r="F55" s="43"/>
+      <c r="G55" s="43"/>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B56" s="12" t="s">

</xml_diff>